<commit_message>
test a few different arimas
</commit_message>
<xml_diff>
--- a/excel/tcc_tabelas.xlsx
+++ b/excel/tcc_tabelas.xlsx
@@ -8,14 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tassi\Documents\Programming\MBA\xchange\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618037DE-11F9-4C7B-A3F4-26FDE1B04121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A1549A-223E-469C-9D96-708AC9A2F558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4C7AE94A-1523-40EC-A6BD-22156EEB7AAF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4C7AE94A-1523-40EC-A6BD-22156EEB7AAF}"/>
   </bookViews>
   <sheets>
     <sheet name="AIC_BIC_LL" sheetId="3" r:id="rId1"/>
     <sheet name="USD_head" sheetId="1" r:id="rId2"/>
     <sheet name="ADF_KPSS_1" sheetId="2" r:id="rId3"/>
+    <sheet name="ADF_KPSS_2" sheetId="5" r:id="rId4"/>
+    <sheet name="Granger" sheetId="4" r:id="rId5"/>
+    <sheet name="AIC_BIC_LL (2)" sheetId="6" r:id="rId6"/>
+    <sheet name="Ljung_Shapiro_Jarque" sheetId="7" r:id="rId7"/>
+    <sheet name="ARIMA_stats" sheetId="9" r:id="rId8"/>
+    <sheet name="RMSE_" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="69">
   <si>
     <t>date</t>
   </si>
@@ -143,6 +149,108 @@
   </si>
   <si>
     <t>Série</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>log(USD) + diff(1)</t>
+  </si>
+  <si>
+    <t>0,1**</t>
+  </si>
+  <si>
+    <t>Nota**: o valor-p real é maior que o retornado pelos testes</t>
+  </si>
+  <si>
+    <t>0,01*</t>
+  </si>
+  <si>
+    <t>Nota*: o valor-p real é menor que o retornado pelos testes pois as estatísticas de teste estão fora da faixa de valores disponíveis</t>
+  </si>
+  <si>
+    <t>Variável</t>
+  </si>
+  <si>
+    <t>USD lag 1</t>
+  </si>
+  <si>
+    <t>USD lag 2</t>
+  </si>
+  <si>
+    <t>USD lag 4</t>
+  </si>
+  <si>
+    <t>USD lag 5</t>
+  </si>
+  <si>
+    <t>USD lag 6</t>
+  </si>
+  <si>
+    <t>USD lag 7</t>
+  </si>
+  <si>
+    <t>Valor-p</t>
+  </si>
+  <si>
+    <t>Lag 1</t>
+  </si>
+  <si>
+    <t>Lag 2</t>
+  </si>
+  <si>
+    <t>Lag 3</t>
+  </si>
+  <si>
+    <t>Lag 4</t>
+  </si>
+  <si>
+    <t>USD lag 3</t>
+  </si>
+  <si>
+    <t>Lag 5</t>
+  </si>
+  <si>
+    <t>F stat</t>
+  </si>
+  <si>
+    <t>Tabela 4. Teste de causalidade de Granger - USD</t>
+  </si>
+  <si>
+    <t>Tabela 3. Valores dos testes ADF e KPSS</t>
+  </si>
+  <si>
+    <t>Tabela 4. Modelos ARIMA escolhidos para predição e comparação</t>
+  </si>
+  <si>
+    <t>Tabela 4. Teste de autocorrelação nos resíduos dos modelos</t>
+  </si>
+  <si>
+    <t>Estatísticas</t>
+  </si>
+  <si>
+    <t>AR(1)</t>
+  </si>
+  <si>
+    <t>MA(1)</t>
+  </si>
+  <si>
+    <t>AR(2)</t>
+  </si>
+  <si>
+    <t>MA(2)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Modelos</t>
+  </si>
+  <si>
+    <t>Ljung</t>
+  </si>
+  <si>
+    <t>Tabela 4. Valores-p para os termos AR(p) e MA(q)</t>
   </si>
 </sst>
 </file>
@@ -150,9 +258,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="172" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -190,7 +298,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -238,11 +346,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -267,32 +384,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -629,33 +791,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ECCAF4-F4B5-4BCC-B95D-1539226F966C}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="19.125" customWidth="1"/>
-    <col min="2" max="2" width="11.625" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="11.75" customWidth="1"/>
+    <col min="2" max="3" width="13.625" customWidth="1"/>
+    <col min="4" max="4" width="13.25" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="9" t="s">
-        <v>18</v>
+      <c r="A2" s="26" t="s">
+        <v>66</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>19</v>
@@ -672,19 +833,19 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="5">
-        <v>-883.24599999999998</v>
+        <v>-885.09500000000003</v>
       </c>
       <c r="C3" s="5">
-        <v>-874.66700000000003</v>
+        <v>-882.23500000000001</v>
       </c>
       <c r="D3" s="5">
-        <v>444.62299999999999</v>
+        <v>443.54700000000003</v>
       </c>
       <c r="E3" s="4">
-        <v>5.9379999999999997E-5</v>
+        <v>6.037E-5</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -706,33 +867,33 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B5" s="5">
-        <v>-885.09500000000003</v>
+        <v>-885.221</v>
       </c>
       <c r="C5" s="5">
-        <v>-882.23500000000001</v>
+        <v>-879.50099999999998</v>
       </c>
       <c r="D5" s="5">
-        <v>443.54700000000003</v>
+        <v>444.61099999999999</v>
       </c>
       <c r="E5" s="4">
-        <v>6.037E-5</v>
+        <v>5.9339999999999998E-5</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="5">
-        <v>-885.221</v>
+        <v>-883.23099999999999</v>
       </c>
       <c r="C6" s="5">
-        <v>-879.50099999999998</v>
+        <v>-874.65</v>
       </c>
       <c r="D6" s="5">
-        <v>444.61099999999999</v>
+        <v>444.61</v>
       </c>
       <c r="E6" s="4">
         <v>5.9339999999999998E-5</v>
@@ -740,61 +901,200 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="5">
-        <v>-883.21400000000006</v>
+        <v>-883.24599999999998</v>
       </c>
       <c r="C7" s="5">
-        <v>-874.63400000000001</v>
+        <v>-874.66700000000003</v>
       </c>
       <c r="D7" s="5">
-        <v>444.60700000000003</v>
+        <v>444.62299999999999</v>
       </c>
       <c r="E7" s="4">
-        <v>5.94E-5</v>
+        <v>5.9379999999999997E-5</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="5">
+        <v>-883.21400000000006</v>
+      </c>
+      <c r="C8" s="5">
+        <v>-874.63400000000001</v>
+      </c>
+      <c r="D8" s="5">
+        <v>444.60700000000003</v>
+      </c>
+      <c r="E8" s="4">
+        <v>5.94E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="1:5" ht="27.75" customHeight="1">
+      <c r="A10" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="29">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.13</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="5">
-        <v>-883.23099999999999</v>
-      </c>
-      <c r="C8" s="5">
-        <v>-874.65</v>
-      </c>
-      <c r="D8" s="5">
-        <v>444.61</v>
-      </c>
-      <c r="E8" s="4">
-        <v>5.9339999999999998E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="13" t="s">
+      <c r="B18" s="6">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0.13</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0.84</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.113</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-    </row>
-    <row r="10" spans="1:5" ht="27.75" customHeight="1">
-      <c r="A10" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A9:E9"/>
     <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A9:E9"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A13:E13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -805,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEBDEFA-26B6-4CF6-AD29-023CB023B6F0}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -819,13 +1119,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
@@ -845,214 +1145,214 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="25">
+      <c r="A3" s="20">
         <v>45375</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="18">
         <v>5.0014500000000002</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="17">
         <v>1.60972787039222</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="16">
         <v>0</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="25">
+      <c r="A4" s="20">
         <v>45376</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="17">
         <v>5.0023499999999999</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="17">
         <v>1.6099078020186901</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="14">
         <v>8.9999999999960001E-4</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="19" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="25">
+      <c r="A5" s="20">
         <v>45377</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="17">
         <v>4.9737</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="17">
         <v>1.60416402993139</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="15">
         <v>-2.8649999999999801E-2</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="25">
+      <c r="A6" s="20">
         <v>45378</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="17">
         <v>4.9771999999999998</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="17">
         <v>1.60486748391933</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="14">
         <v>3.4999999999998001E-3</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="25">
+      <c r="A7" s="20">
         <v>45379</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="17">
         <v>4.9923500000000001</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="17">
         <v>1.6079067407888701</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="15">
         <v>1.51500000000002E-2</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="25">
+      <c r="A8" s="20">
         <v>45380</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="17">
         <v>5.01525</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="17">
         <v>1.61248327062006</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="14">
         <v>2.28999999999999E-2</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="25">
+      <c r="A9" s="20">
         <v>45381</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="17">
         <v>5.01525</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="17">
         <v>1.61248327062006</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="16">
         <v>0</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="19" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="25">
+      <c r="A10" s="20">
         <v>45382</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="17">
         <v>5.01525</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="17">
         <v>1.61248327062006</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="16">
         <v>0</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="25">
+      <c r="A11" s="20">
         <v>45383</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="17">
         <v>5.0149499999999998</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="17">
         <v>1.61242345127446</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="14">
         <v>-3.0000000000009999E-4</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="19" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="25">
+      <c r="A12" s="20">
         <v>45384</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="17">
         <v>5.0551000000000004</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="17">
         <v>1.6203976346704301</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="15">
         <v>4.0150000000000498E-2</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
     </row>
     <row r="17" spans="4:4">
-      <c r="D17" s="16"/>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="4:4">
-      <c r="D18" s="17"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="19" spans="4:4">
-      <c r="D19" s="17"/>
+      <c r="D19" s="13"/>
     </row>
     <row r="20" spans="4:4">
-      <c r="D20" s="17"/>
+      <c r="D20" s="13"/>
     </row>
     <row r="21" spans="4:4">
-      <c r="D21" s="17"/>
+      <c r="D21" s="13"/>
     </row>
     <row r="22" spans="4:4">
-      <c r="D22" s="17"/>
+      <c r="D22" s="13"/>
     </row>
     <row r="23" spans="4:4">
-      <c r="D23" s="17"/>
+      <c r="D23" s="13"/>
     </row>
     <row r="24" spans="4:4">
-      <c r="D24" s="17"/>
+      <c r="D24" s="13"/>
     </row>
     <row r="25" spans="4:4">
-      <c r="D25" s="17"/>
+      <c r="D25" s="13"/>
     </row>
     <row r="26" spans="4:4">
-      <c r="D26" s="17"/>
+      <c r="D26" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1065,29 +1365,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B818D3E-78E0-45F8-A90F-07C838886677}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:E4"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="3" width="15.375" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="12.25" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
     <col min="5" max="5" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="11" t="s">
         <v>34</v>
       </c>
@@ -1103,8 +1408,17 @@
       <c r="E2" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1120,8 +1434,17 @@
       <c r="E3" s="6">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="23">
+        <v>-446.8</v>
+      </c>
+      <c r="G3" s="23">
+        <v>-438.3</v>
+      </c>
+      <c r="H3" s="23">
+        <v>226.42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
@@ -1130,11 +1453,872 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
+    <row r="18" spans="5:6" ht="14.25" customHeight="1">
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" spans="5:6">
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B669F3FC-58BB-4F0A-A6C8-CB9E62B5A962}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="3" width="15.375" customWidth="1"/>
+    <col min="4" max="4" width="19.875" customWidth="1"/>
+    <col min="5" max="5" width="15.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6">
+        <v>-1.895</v>
+      </c>
+      <c r="C3" s="6">
+        <v>-1.915</v>
+      </c>
+      <c r="D3">
+        <v>-8.8559999999999999</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.522E-14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1.7030000000000001</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1.7070000000000001</v>
+      </c>
+      <c r="D5">
+        <v>0.123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="6">
+        <v>-446.8</v>
+      </c>
+      <c r="C7" s="6">
+        <v>-880.3</v>
+      </c>
+      <c r="D7">
+        <v>-462.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6">
+        <v>-438.3</v>
+      </c>
+      <c r="C8" s="6">
+        <v>-871.8</v>
+      </c>
+      <c r="D8">
+        <v>-454</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="6">
+        <v>226.42</v>
+      </c>
+      <c r="C9" s="6">
+        <v>443.17</v>
+      </c>
+      <c r="D9">
+        <v>234.29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="39"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A11:D12"/>
+    <mergeCell ref="A10:D10"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82451294-0A52-4E7E-B5DB-C85CCA778691}">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="7.875" customWidth="1"/>
+    <col min="3" max="3" width="8.125" customWidth="1"/>
+    <col min="4" max="4" width="8.25" customWidth="1"/>
+    <col min="5" max="5" width="7.75" customWidth="1"/>
+    <col min="6" max="6" width="8.25" customWidth="1"/>
+    <col min="7" max="7" width="7.75" customWidth="1"/>
+    <col min="8" max="9" width="7.625" customWidth="1"/>
+    <col min="10" max="10" width="7.375" customWidth="1"/>
+    <col min="11" max="11" width="7.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="B2" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="41"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <v>3.0968</v>
+      </c>
+      <c r="C4">
+        <v>8.09E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.16039999999999999</v>
+      </c>
+      <c r="E4">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="F4">
+        <v>0.13739999999999999</v>
+      </c>
+      <c r="G4">
+        <v>0.9375</v>
+      </c>
+      <c r="H4">
+        <v>0.66569999999999996</v>
+      </c>
+      <c r="I4">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="J4">
+        <v>0.16869999999999999</v>
+      </c>
+      <c r="K4">
+        <v>0.97360000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <v>0.17560000000000001</v>
+      </c>
+      <c r="C5">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="D5">
+        <v>0.36459999999999998</v>
+      </c>
+      <c r="E5">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="F5">
+        <v>1.0273000000000001</v>
+      </c>
+      <c r="G5">
+        <v>0.38319999999999999</v>
+      </c>
+      <c r="H5">
+        <v>0.87050000000000005</v>
+      </c>
+      <c r="I5">
+        <v>0.4839</v>
+      </c>
+      <c r="J5">
+        <v>0.21</v>
+      </c>
+      <c r="K5">
+        <v>0.9577</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6">
+        <v>0.93559999999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.33529999999999999</v>
+      </c>
+      <c r="D6">
+        <v>1.696</v>
+      </c>
+      <c r="E6">
+        <v>0.18779999999999999</v>
+      </c>
+      <c r="F6">
+        <v>1.29</v>
+      </c>
+      <c r="G6">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="H6">
+        <v>0.86050000000000004</v>
+      </c>
+      <c r="I6">
+        <v>0.49</v>
+      </c>
+      <c r="J6">
+        <v>0.28760000000000002</v>
+      </c>
+      <c r="K6">
+        <v>0.91900000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <v>2.6953</v>
+      </c>
+      <c r="C7">
+        <v>0.1032</v>
+      </c>
+      <c r="D7">
+        <v>1.9248000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.15040000000000001</v>
+      </c>
+      <c r="F7">
+        <v>1.1793</v>
+      </c>
+      <c r="G7">
+        <v>0.32079999999999997</v>
+      </c>
+      <c r="H7">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="I7">
+        <v>0.4385</v>
+      </c>
+      <c r="J7">
+        <v>0.27739999999999998</v>
+      </c>
+      <c r="K7">
+        <v>0.92459999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8">
+        <v>1.8823000000000001</v>
+      </c>
+      <c r="C8">
+        <v>0.1726</v>
+      </c>
+      <c r="D8">
+        <v>1.0189999999999999</v>
+      </c>
+      <c r="E8">
+        <v>0.36409999999999998</v>
+      </c>
+      <c r="F8">
+        <v>0.74</v>
+      </c>
+      <c r="G8">
+        <v>0.53029999999999999</v>
+      </c>
+      <c r="H8">
+        <v>0.4975</v>
+      </c>
+      <c r="I8">
+        <v>0.73760000000000003</v>
+      </c>
+      <c r="J8">
+        <v>0.26690000000000003</v>
+      </c>
+      <c r="K8">
+        <v>0.93030000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF304062-703C-4CBE-BA0B-A149038AF557}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="13.875" customWidth="1"/>
+    <col min="4" max="4" width="14.75" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5">
+        <v>-885.09500000000003</v>
+      </c>
+      <c r="C3" s="5">
+        <v>-882.23500000000001</v>
+      </c>
+      <c r="D3" s="5">
+        <v>443.54700000000003</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6.037E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5">
+        <v>-885.20600000000002</v>
+      </c>
+      <c r="C4" s="5">
+        <v>-879.48699999999997</v>
+      </c>
+      <c r="D4" s="5">
+        <v>444.60300000000001</v>
+      </c>
+      <c r="E4" s="4">
+        <v>5.9330000000000003E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5">
+        <v>-885.221</v>
+      </c>
+      <c r="C5" s="5">
+        <v>-879.50099999999998</v>
+      </c>
+      <c r="D5" s="5">
+        <v>444.61099999999999</v>
+      </c>
+      <c r="E5" s="4">
+        <v>5.9339999999999998E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+    </row>
+    <row r="7" spans="1:6" ht="28.5" customHeight="1">
+      <c r="A7" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+    </row>
+    <row r="10" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A10" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A12" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="29">
+        <v>-885.09500000000003</v>
+      </c>
+      <c r="C12" s="29">
+        <v>-885.20600000000002</v>
+      </c>
+      <c r="D12" s="29">
+        <v>-885.221</v>
+      </c>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A13" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="29">
+        <v>-882.23500000000001</v>
+      </c>
+      <c r="C13" s="29">
+        <v>-879.48699999999997</v>
+      </c>
+      <c r="D13" s="29">
+        <v>-879.50099999999998</v>
+      </c>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="29">
+        <v>443.54700000000003</v>
+      </c>
+      <c r="C14" s="29">
+        <v>444.60300000000001</v>
+      </c>
+      <c r="D14" s="29">
+        <v>444.61099999999999</v>
+      </c>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="30">
+        <v>6.037E-5</v>
+      </c>
+      <c r="C15" s="30">
+        <v>5.9330000000000003E-5</v>
+      </c>
+      <c r="D15" s="30">
+        <v>5.9339999999999998E-5</v>
+      </c>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A10:E10"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0E06F8-CD60-413A-808E-EBFB68A5C580}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="10.875" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="9"/>
+      <c r="B2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5">
+        <v>-885.09500000000003</v>
+      </c>
+      <c r="C3" s="5">
+        <v>-882.23500000000001</v>
+      </c>
+      <c r="D3" s="5">
+        <v>443.54700000000003</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6.037E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5">
+        <v>-885.20600000000002</v>
+      </c>
+      <c r="C4" s="5">
+        <v>-879.48699999999997</v>
+      </c>
+      <c r="D4" s="5">
+        <v>444.60300000000001</v>
+      </c>
+      <c r="E4" s="4">
+        <v>5.9330000000000003E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{257EAAC2-2875-4FFA-8C8D-19621318FF10}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD36E46-958F-477D-BA6A-BEFC826D32CC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>